<commit_message>
backup before use the imp_th_process
</commit_message>
<xml_diff>
--- a/DAISY-git/build/Daisy1206/input/输入卡.xlsx
+++ b/DAISY-git/build/Daisy1206/input/输入卡.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>height</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -263,6 +263,14 @@
   </si>
   <si>
     <t>这个初始压力给定是pguess函数的pin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ny_start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ny_end</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -369,7 +377,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -386,6 +394,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -397,9 +412,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="G4:L26"/>
+  <dimension ref="G4:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -796,7 +808,7 @@
       </c>
     </row>
     <row r="5" spans="7:11">
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -813,7 +825,7 @@
       </c>
     </row>
     <row r="6" spans="7:11">
-      <c r="G6" s="7"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="1" t="s">
         <v>28</v>
       </c>
@@ -828,7 +840,7 @@
       </c>
     </row>
     <row r="7" spans="7:11">
-      <c r="G7" s="7"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="1" t="s">
         <v>29</v>
       </c>
@@ -843,13 +855,11 @@
       </c>
     </row>
     <row r="8" spans="7:11">
-      <c r="G8" s="7"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="2">
-        <v>5.0000000000000001E-4</v>
-      </c>
+      <c r="I8" s="2"/>
       <c r="J8" s="1" t="s">
         <v>52</v>
       </c>
@@ -858,7 +868,7 @@
       </c>
     </row>
     <row r="9" spans="7:11">
-      <c r="G9" s="7"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="1" t="s">
         <v>32</v>
       </c>
@@ -873,7 +883,7 @@
       </c>
     </row>
     <row r="10" spans="7:11">
-      <c r="G10" s="7"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,7 +898,7 @@
       </c>
     </row>
     <row r="11" spans="7:11">
-      <c r="G11" s="7"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="1" t="s">
         <v>58</v>
       </c>
@@ -901,7 +911,7 @@
       </c>
     </row>
     <row r="12" spans="7:11">
-      <c r="G12" s="8"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="1" t="s">
         <v>1</v>
       </c>
@@ -916,7 +926,7 @@
       </c>
     </row>
     <row r="13" spans="7:11">
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -933,7 +943,7 @@
       </c>
     </row>
     <row r="14" spans="7:11">
-      <c r="G14" s="7"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="1" t="s">
         <v>3</v>
       </c>
@@ -948,7 +958,7 @@
       </c>
     </row>
     <row r="15" spans="7:11">
-      <c r="G15" s="7"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="1" t="s">
         <v>4</v>
       </c>
@@ -963,88 +973,80 @@
       </c>
     </row>
     <row r="16" spans="7:11">
-      <c r="G16" s="8"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I16" s="2">
         <v>10</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="7:12">
+      <c r="G17" s="9"/>
+      <c r="H17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="7:12">
+      <c r="G18" s="10"/>
+      <c r="H18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="6">
+        <v>10</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="7:12">
-      <c r="G17" s="1" t="s">
+    <row r="19" spans="7:12">
+      <c r="G19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I19" s="2">
         <v>0.03</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="7:12">
-      <c r="G18" s="5" t="s">
+    <row r="20" spans="7:12">
+      <c r="G20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I20" s="2">
         <v>493</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="7:12">
-      <c r="G19" s="5"/>
-      <c r="H19" s="1" t="s">
+    <row r="21" spans="7:12">
+      <c r="G21" s="7"/>
+      <c r="H21" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="I19" s="2">
-        <v>10000</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="7:12">
-      <c r="G20" s="5"/>
-      <c r="H20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="2">
-        <v>2</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="7:12">
-      <c r="G21" s="5"/>
-      <c r="H21" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="I21" s="2">
         <v>10000</v>
@@ -1053,98 +1055,128 @@
         <v>56</v>
       </c>
       <c r="K21" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="7:12">
+      <c r="G22" s="7"/>
+      <c r="H22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="7:12">
+      <c r="G23" s="7"/>
+      <c r="H23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="7:12">
-      <c r="G22" s="5" t="s">
+    <row r="24" spans="7:12">
+      <c r="G24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I24" s="2">
         <v>493</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="7:12">
-      <c r="G23" s="5"/>
-      <c r="H23" s="1" t="s">
+    <row r="25" spans="7:12">
+      <c r="G25" s="7"/>
+      <c r="H25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I25" s="2">
         <v>2</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="7:12">
-      <c r="G24" s="5"/>
-      <c r="H24" s="1" t="s">
+    <row r="26" spans="7:12">
+      <c r="G26" s="7"/>
+      <c r="H26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I26" s="2">
         <v>60000</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L24" s="9" t="s">
+      <c r="L26" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="7:12">
-      <c r="G25" s="5" t="s">
+    <row r="27" spans="7:12">
+      <c r="G27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I27" s="2">
         <v>1E-3</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="7:12">
-      <c r="G26" s="5"/>
-      <c r="H26" s="1" t="s">
+    <row r="28" spans="7:12">
+      <c r="G28" s="7"/>
+      <c r="H28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I28" s="2">
         <v>0.1</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="G27:G28"/>
     <mergeCell ref="G5:G12"/>
-    <mergeCell ref="G13:G16"/>
+    <mergeCell ref="G13:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>